<commit_message>
checkpoint before restrucadding output data to folder
</commit_message>
<xml_diff>
--- a/Results/Activity Summary Notes.xlsx
+++ b/Results/Activity Summary Notes.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -59,12 +56,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -362,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L106"/>
+  <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,11 +414,6 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Record Date</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
           <t>Old Production Summary</t>
         </is>
       </c>
@@ -468,13 +459,10 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Anderson O&amp;G paid between $2/acre and $640/acre, averaging at $184/acre per section.  Diamond Resources paid $8/acre.  The average price in 2019 overall within the 3 radius was $145/acre.</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L2" t="inlineStr">
+Anderson O&amp;G paid $2/acre.  Diamond Resources paid $8/acre.  The average price in 2019 overall within the 3 radius was $145/acre.  The highest price paid in 2019 was $640/acre</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -521,13 +509,10 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Southland Royalty paid between $39/acre and $46/acre, averaging at $42/acre per section.  The average price in 2018 overall within the 3 radius was $42/acre.</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L3" t="inlineStr">
+Southland Royalty paid $39/acre.  The average price in 2018 overall within the 3 radius was $42/acre.  The highest price paid in 2018 was $46/acre</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -578,14 +563,10 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Western American Resources paid $640/acre.  </t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L4" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -632,13 +613,10 @@
       <c r="J5" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Edge Energy Ii paid between $53/acre and $106/acre, averaging at $85/acre per section.  Gungnir Resources paid between $111/acre and $49280/acre, averaging at $16547/acre per section.  The average price in 2019 overall within the 3 radius was $5861/acre.</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L5" t="inlineStr">
+Edge Energy Ii paid between $53/acre and $106/acre, averaging at $85/acre per section.  Carpenter &amp; Sons paid between $1760/acre and $8960/acre, averaging at $4373/acre per section.  The average price in 2019 overall within the 3 radius was $5861/acre.  The highest price paid in 2019 was $49280/acre</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -684,14 +662,10 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Midland Energy paid $21/acre.  </t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L6" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -737,14 +711,10 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Robert L Bayless paid $52/acre.  The average price in 2017 overall within the 3 radius was $52/acre.</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L7" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -790,14 +760,10 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Midland Energy paid $28/acre.  </t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L8" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -844,13 +810,10 @@
       <c r="J9" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Robert L Bayless paid between $26/acre and $52/acre, averaging at $44/acre per section.  The average price in 2017 overall within the 3 radius was $44/acre.</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L9" t="inlineStr">
+Robert L Bayless paid between $26/acre and $28/acre, averaging at $27/acre per section.  The average price in 2017 overall within the 3 radius was $44/acre.  The highest price paid in 2017 was $52/acre</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -896,14 +859,10 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Midland Energy paid $28/acre.  </t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L10" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -949,14 +908,10 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Midland Energy paid $28/acre.  </t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L11" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1002,14 +957,10 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Robert L Bayless paid $8/acre.  </t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L12" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1055,14 +1006,10 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Robert L Bayless paid $8/acre.  </t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L13" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1109,13 +1056,10 @@
       <c r="J14" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Colorado Energy Minerals paid $37/acre.  Thunder Basin Resources paid $52/acre.  </t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L14" t="inlineStr">
+Colorado Energy Minerals paid $37/acre.  </t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1161,14 +1105,10 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Colorado Energy Minerals paid $37/acre.  </t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L15" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1215,13 +1155,10 @@
       <c r="J16" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Colorado Energy Minerals paid $37/acre.  Thunder Basin Resources paid $52/acre.  </t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L16" t="inlineStr">
+Colorado Energy Minerals paid $37/acre.  </t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1272,13 +1209,10 @@
       <c r="J17" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Rockies Resources Holding paid between $10320/acre and $30960/acre, averaging at $20640/acre per section.  Massif O&amp;G paid $133120/acre.  The average price in 2019 overall within the 3 radius was $58133/acre.</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L17" t="inlineStr">
+Rockies Resources Holding paid between $10320/acre and $30960/acre, averaging at $20640/acre per section.  The average price in 2019 overall within the 3 radius was $58133/acre.  The highest price paid in 2019 was $133120/acre</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1330,14 +1264,10 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2014.
-Mbi O&amp;G paid $3100/acre.  </t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L18" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1389,14 +1319,10 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2014.
-Mbi O&amp;G paid $3100/acre.  </t>
-        </is>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L19" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1448,14 +1374,10 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Peak Powder River Resources paid $4002/acre.  </t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L20" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1507,14 +1429,10 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L21" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1566,14 +1484,10 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L22" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1625,14 +1539,10 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L23" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1684,14 +1594,10 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K24" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L24" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1743,14 +1649,10 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L25" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1802,14 +1704,10 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L26" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1861,14 +1759,10 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L27" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1920,14 +1814,10 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K28" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L28" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -1979,14 +1869,10 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K29" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L29" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2038,14 +1924,10 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Onyx Energy paid $3052/acre.  </t>
-        </is>
-      </c>
-      <c r="K30" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L30" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2092,13 +1974,10 @@
       <c r="J31" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Whiskey Gulch paid between $83/acre and $708/acre, averaging at $291/acre per section.  Langham Petr paid $208/acre.  The average price in 2019 overall within the 3 radius was $263/acre.</t>
-        </is>
-      </c>
-      <c r="K31" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L31" t="inlineStr">
+Whiskey Gulch paid $83/acre.  Langham Petr paid $208/acre.  The average price in 2019 overall within the 3 radius was $263/acre.  The highest price paid in 2019 was $708/acre</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2149,13 +2028,10 @@
       <c r="J32" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Renos L&amp;M paid $506/acre.  Baseline Minerals paid between $1101/acre and $1514/acre, averaging at $1308/acre per section.  The average price in 2019 overall within the 3 radius was $777/acre.</t>
-        </is>
-      </c>
-      <c r="K32" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L32" t="inlineStr">
+Renos L&amp;M paid $506/acre.  Baseline Minerals paid $1101/acre.  The average price in 2019 overall within the 3 radius was $777/acre.  The highest price paid in 2019 was $1514/acre</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2202,13 +2078,10 @@
       <c r="J33" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Stroud Expl paid $30/acre.  Kirkwood O&amp;G paid $16/acre.  The average price in 2017 overall within the 3 radius was $25/acre.</t>
-        </is>
-      </c>
-      <c r="K33" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L33" t="inlineStr">
+Kirkwood O&amp;G paid $16/acre.  The average price in 2017 overall within the 3 radius was $25/acre.  The highest price paid in 2017 was $30/acre</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2261,13 +2134,10 @@
       <c r="J34" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Samson Resources paid $1526/acre.  The average price in 2019 overall within the 3 radius was $2080/acre.</t>
-        </is>
-      </c>
-      <c r="K34" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L34" t="inlineStr">
+2323 Ss paid $302/acre.  Samson Resources paid $1526/acre.  The average price in 2019 overall within the 3 radius was $2080/acre.  The highest price paid in 2019 was $5751/acre</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2320,13 +2190,10 @@
       <c r="J35" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Titan Expl paid $5751/acre.  The average price in 2019 overall within the 3 radius was $2150/acre.</t>
-        </is>
-      </c>
-      <c r="K35" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L35" t="inlineStr">
+2323 Ss paid $302/acre.  Colorado Energy Minerals paid $2011/acre.  The average price in 2019 overall within the 3 radius was $2150/acre.  The highest price paid in 2019 was $5751/acre</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2377,13 +2244,10 @@
       <c r="J36" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Titan Expl paid $5751/acre.  The average price in 2019 overall within the 3 radius was $2150/acre.</t>
-        </is>
-      </c>
-      <c r="K36" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L36" t="inlineStr">
+2323 Ss paid $302/acre.  Colorado Energy Minerals paid $2011/acre.  The average price in 2019 overall within the 3 radius was $2150/acre.  The highest price paid in 2019 was $5751/acre</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2434,13 +2298,10 @@
       <c r="J37" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Titan Expl paid $5751/acre.  2323 Ss paid $302/acre.  The average price in 2019 overall within the 3 radius was $3013/acre.</t>
-        </is>
-      </c>
-      <c r="K37" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L37" t="inlineStr">
+2323 Ss paid $302/acre.  Colorado Energy Minerals paid $2011/acre.  The average price in 2019 overall within the 3 radius was $3013/acre.  The highest price paid in 2019 was $5751/acre</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2492,14 +2353,10 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2013.
-Lone Tree Energy paid $570/acre.  </t>
-        </is>
-      </c>
-      <c r="K38" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L38" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2551,14 +2408,10 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2010.
-Southwestern Prod paid $700/acre.  </t>
-        </is>
-      </c>
-      <c r="K39" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L39" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2605,13 +2458,10 @@
       <c r="J40" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Impact Energy paid $502/acre.  Knprb Leases paid $27/acre.  The average price in 2019 overall within the 3 radius was $366/acre.</t>
-        </is>
-      </c>
-      <c r="K40" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L40" t="inlineStr">
+Knprb Leases paid $27/acre.  The average price in 2019 overall within the 3 radius was $366/acre.  The highest price paid in 2019 was $502/acre</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2658,13 +2508,10 @@
       <c r="J41" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Impact Energy paid $502/acre.  Knprb Leases paid between $27/acre and $252/acre, averaging at $177/acre per section.  The average price in 2019 overall within the 3 radius was $284/acre.</t>
-        </is>
-      </c>
-      <c r="K41" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L41" t="inlineStr">
+Knprb Leases paid between $27/acre and $252/acre, averaging at $177/acre per section.  Bradley Williams paid $7/acre.  The average price in 2019 overall within the 3 radius was $284/acre.  The highest price paid in 2019 was $502/acre</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2711,13 +2558,10 @@
       <c r="J42" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Percheron Professional Services paid $59/acre.  Kirkwood Resources paid $84/acre.  The average price in 2019 overall within the 3 radius was $67/acre.</t>
-        </is>
-      </c>
-      <c r="K42" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L42" t="inlineStr">
+Percheron Professional Services paid $59/acre.  The average price in 2019 overall within the 3 radius was $67/acre.  The highest price paid in 2019 was $84/acre</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2763,14 +2607,10 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid $2/acre.  The average price in 2019 overall within the 3 radius was $2/acre.</t>
-        </is>
-      </c>
-      <c r="K43" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L43" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -2817,13 +2657,10 @@
       <c r="J44" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Mason Resources paid $788/acre.  Rockies Resources Holding paid $640/acre.  </t>
-        </is>
-      </c>
-      <c r="K44" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L44" t="inlineStr">
+Rockies Resources Holding paid $640/acre.  </t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 22 wells outside the tract within a 3 mile radius.
@@ -2872,14 +2709,10 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2016.
-Angelle &amp; Donohue O&amp;G paid $10/acre.  </t>
-        </is>
-      </c>
-      <c r="K45" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L45" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -2927,13 +2760,10 @@
       <c r="J46" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid between $2/acre and $12/acre, averaging at $7/acre per section.  Diamond Resources paid $19/acre.  The average price in 2019 overall within the 3 radius was $11/acre.</t>
-        </is>
-      </c>
-      <c r="K46" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L46" t="inlineStr">
+Kirkwood Resources paid between $2/acre and $12/acre, averaging at $7/acre per section.  The average price in 2019 overall within the 3 radius was $11/acre.  The highest price paid in 2019 was $19/acre</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 1 wells outside the tract within a 3 mile radius.
@@ -2983,13 +2813,10 @@
       <c r="J47" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $12/acre.  Sitka O&amp;G paid $18/acre.  </t>
-        </is>
-      </c>
-      <c r="K47" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L47" t="inlineStr">
+Kirkwood Resources paid $12/acre.  </t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 2 wells outside the tract within a 3 mile radius.
@@ -3039,13 +2866,10 @@
       <c r="J48" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Baseline Minerals paid between $22/acre and $23/acre, averaging at $22/acre per section.  The average price in 2018 overall within the 3 radius was $22/acre.</t>
-        </is>
-      </c>
-      <c r="K48" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L48" t="inlineStr">
+Baseline Minerals paid $22/acre.  The average price in 2018 overall within the 3 radius was $22/acre.  The highest price paid in 2018 was $23/acre</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -3091,14 +2915,10 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Kirkwood O&amp;G paid $16/acre.  </t>
-        </is>
-      </c>
-      <c r="K49" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L49" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -3144,14 +2964,10 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Kirkwood O&amp;G paid $16/acre.  </t>
-        </is>
-      </c>
-      <c r="K50" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L50" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -3197,14 +3013,10 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $12/acre.  </t>
-        </is>
-      </c>
-      <c r="K51" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L51" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -3251,14 +3063,10 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Rockies Resources Holding paid $29/acre.  </t>
-        </is>
-      </c>
-      <c r="K52" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L52" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -3304,14 +3112,10 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Hrm Resources paid $19/acre.  </t>
-        </is>
-      </c>
-      <c r="K53" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L53" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
         <is>
           <t xml:space="preserve">There are 1 wells within the tract.
 1 wells reported production. They produced: 16 mbbl and 734 mmcf at 12145 ft from years 2006-2019
@@ -3364,13 +3168,10 @@
       <c r="J54" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Shadco paid between $2/acre and $7/acre, averaging at $4/acre per section.  The average price in 2019 overall within the 3 radius was $4/acre.</t>
-        </is>
-      </c>
-      <c r="K54" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L54" t="inlineStr">
+Shadco paid $2/acre.  The average price in 2019 overall within the 3 radius was $4/acre.  The highest price paid in 2019 was $7/acre</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -3417,13 +3218,10 @@
       <c r="J55" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Mason Resources paid between $71/acre and $81/acre, averaging at $77/acre per section.  The average price in 2019 overall within the 3 radius was $77/acre.</t>
-        </is>
-      </c>
-      <c r="K55" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L55" t="inlineStr">
+Mason Resources paid between $71/acre and $76/acre, averaging at $75/acre per section.  The average price in 2019 overall within the 3 radius was $77/acre.  The highest price paid in 2019 was $81/acre</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -3470,13 +3268,10 @@
       <c r="J56" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Prima Expl paid between $23/acre and $52/acre, averaging at $38/acre per section.  </t>
-        </is>
-      </c>
-      <c r="K56" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L56" t="inlineStr">
+Prima Expl paid $23/acre.  </t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -3528,14 +3323,10 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bso paid $152/acre.  </t>
-        </is>
-      </c>
-      <c r="K57" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L57" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -3582,13 +3373,10 @@
       <c r="J58" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Black Oak Energy paid between $18/acre and $58/acre, averaging at $25/acre per section.  The average price in 2018 overall within the 3 radius was $25/acre.</t>
-        </is>
-      </c>
-      <c r="K58" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L58" t="inlineStr">
+Black Oak Energy paid between $18/acre and $28/acre, averaging at $21/acre per section.  The average price in 2018 overall within the 3 radius was $25/acre.  The highest price paid in 2018 was $58/acre</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 3 wells outside the tract within a 3 mile radius.
@@ -3637,14 +3425,10 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Black Oak Energy paid $50/acre.  The average price in 2019 overall within the 3 radius was $50/acre.</t>
-        </is>
-      </c>
-      <c r="K59" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L59" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -3691,13 +3475,10 @@
       <c r="J60" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Black Oak Energy paid $50/acre.  Kirkwood Resources paid $26/acre.  The average price in 2019 overall within the 3 radius was $38/acre.</t>
-        </is>
-      </c>
-      <c r="K60" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L60" t="inlineStr">
+Kirkwood Resources paid $26/acre.  The average price in 2019 overall within the 3 radius was $38/acre.  The highest price paid in 2019 was $50/acre</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 19 wells outside the tract within a 3 mile radius.
@@ -3747,13 +3528,10 @@
       <c r="J61" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Black Oak Energy paid $50/acre.  Kirkwood Resources paid $26/acre.  The average price in 2019 overall within the 3 radius was $38/acre.</t>
-        </is>
-      </c>
-      <c r="K61" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L61" t="inlineStr">
+Kirkwood Resources paid $26/acre.  The average price in 2019 overall within the 3 radius was $38/acre.  The highest price paid in 2019 was $50/acre</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -3800,13 +3578,10 @@
       <c r="J62" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Diamond Resources paid $9/acre.  Mason Resources paid $82/acre.  The average price in 2019 overall within the 3 radius was $29/acre.</t>
-        </is>
-      </c>
-      <c r="K62" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L62" t="inlineStr">
+Diamond Resources paid $9/acre.  Kirkwood Resources paid $3/acre.  The average price in 2019 overall within the 3 radius was $29/acre.  The highest price paid in 2019 was $82/acre</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -3852,14 +3627,10 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Diamond Resources paid $9/acre.  The average price in 2019 overall within the 3 radius was $9/acre.</t>
-        </is>
-      </c>
-      <c r="K63" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L63" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 15 wells outside the tract within a 3 mile radius.
@@ -3910,13 +3681,10 @@
       <c r="J64" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Mason Resources paid $76/acre.  Kirkwood O&amp;G paid $19/acre.  The average price in 2019 overall within the 3 radius was $57/acre.</t>
-        </is>
-      </c>
-      <c r="K64" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L64" t="inlineStr">
+Kirkwood O&amp;G paid $19/acre.  The average price in 2019 overall within the 3 radius was $57/acre.  The highest price paid in 2019 was $76/acre</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 33 wells outside the tract within a 3 mile radius.
@@ -3961,7 +3729,7 @@
       <c r="I65" t="inlineStr">
         <is>
           <t xml:space="preserve">There are 4 wells within 3 mile radius that have started producing within last 4 years
-2 are D wells; 2 are V wells
+2 are V wells; 2 are D wells
 1 well has made nan mbbl and 51 mmcfd in 12 months and is currently making nan bpd and 96 mcfd.  2 wells have produced for 25 to 36 months and have made between 0 to 6 mbbls with 31 to 515 mmcf of gas.  These wells are currently averaging 1 bpd and 143 mcfd.  </t>
         </is>
       </c>
@@ -3970,10 +3738,7 @@
           <t>There are no recorded leases within a 3 mile radius</t>
         </is>
       </c>
-      <c r="K65" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L65" t="inlineStr">
+      <c r="K65" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4020,13 +3785,10 @@
       <c r="J66" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $3/acre.  Diamond Resources paid $9/acre.  The average price in 2019 overall within the 3 radius was $17/acre.</t>
-        </is>
-      </c>
-      <c r="K66" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L66" t="inlineStr">
+Kirkwood Resources paid $3/acre.  Diamond Resources paid $9/acre.  The average price in 2019 overall within the 3 radius was $17/acre.  The highest price paid in 2019 was $82/acre</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4072,14 +3834,10 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Black Oak Energy paid $53/acre.  </t>
-        </is>
-      </c>
-      <c r="K67" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L67" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 4 wells outside the tract within a 3 mile radius.
@@ -4129,13 +3887,10 @@
       <c r="J68" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Hrm Resources paid $62/acre.  Black Oak Energy paid between $52/acre and $53/acre, averaging at $53/acre per section.  The average price in 2019 overall within the 3 radius was $54/acre.</t>
-        </is>
-      </c>
-      <c r="K68" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L68" t="inlineStr">
+Black Oak Energy paid between $52/acre and $53/acre, averaging at $53/acre per section.  Mason Resources paid $27/acre.  The average price in 2019 overall within the 3 radius was $54/acre.  The highest price paid in 2019 was $62/acre</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4181,14 +3936,10 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid $16/acre.  </t>
-        </is>
-      </c>
-      <c r="K69" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L69" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4235,13 +3986,10 @@
       <c r="J70" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Southland Royalty paid between $39/acre and $108/acre, averaging at $78/acre per section.  Baseline Minerals paid between $62/acre and $82/acre, averaging at $72/acre per section.  The average price in 2018 overall within the 3 radius was $77/acre.</t>
-        </is>
-      </c>
-      <c r="K70" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L70" t="inlineStr">
+Southland Royalty paid between $39/acre and $68/acre, averaging at $55/acre per section.  Baseline Minerals paid between $62/acre and $82/acre, averaging at $72/acre per section.  The average price in 2018 overall within the 3 radius was $77/acre.  The highest price paid in 2018 was $108/acre</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
         <is>
           <t xml:space="preserve">There are 3 wells within the tract.
 1 dry holes in tract.
@@ -4293,13 +4041,10 @@
       <c r="J71" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid between $28/acre and $39/acre, averaging at $32/acre per section.  Black Oak Energy paid between $50/acre and $52/acre, averaging at $51/acre per section.  The average price in 2019 overall within the 3 radius was $40/acre.</t>
-        </is>
-      </c>
-      <c r="K71" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L71" t="inlineStr">
+Liberty Petr paid between $28/acre and $39/acre, averaging at $32/acre per section.  Black Oak Energy paid $50/acre.  The average price in 2019 overall within the 3 radius was $40/acre.  The highest price paid in 2019 was $52/acre</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 11 wells outside the tract within a 3 mile radius.
@@ -4351,13 +4096,10 @@
       <c r="J72" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Southland Royalty paid between $36/acre and $67/acre, averaging at $45/acre per section.  Baseline Minerals paid $94/acre.  The average price in 2018 overall within the 3 radius was $57/acre.</t>
-        </is>
-      </c>
-      <c r="K72" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L72" t="inlineStr">
+Southland Royalty paid between $36/acre and $67/acre, averaging at $45/acre per section.  The average price in 2018 overall within the 3 radius was $57/acre.  The highest price paid in 2018 was $94/acre</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
         <is>
           <t xml:space="preserve">There are 1 wells within the tract.
 1 wells reported production. They produced: 11 mbbl and 3659 mmcf at 6579 ft from years 1974-2016
@@ -4407,14 +4149,10 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $2/acre.  </t>
-        </is>
-      </c>
-      <c r="K73" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L73" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4460,14 +4198,10 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2014.
-Teton Resources paid $18/acre.  </t>
-        </is>
-      </c>
-      <c r="K74" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L74" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
         <is>
           <t xml:space="preserve">There are 1 wells within the tract.
 1 wells reported production. They produced: 0 mbbl and 374 mmcf at 11450 ft from years 2002-2018
@@ -4518,13 +4252,10 @@
       <c r="J75" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Black Oak Energy paid between $11/acre and $24/acre, averaging at $17/acre per section.  The average price in 2018 overall within the 3 radius was $17/acre.</t>
-        </is>
-      </c>
-      <c r="K75" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L75" t="inlineStr">
+Black Oak Energy paid between $11/acre and $12/acre, averaging at $12/acre per section.  The average price in 2018 overall within the 3 radius was $17/acre.  The highest price paid in 2018 was $24/acre</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 1 wells outside the tract within a 3 mile radius.
@@ -4574,13 +4305,10 @@
       <c r="J76" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid between $12/acre and $22/acre, averaging at $19/acre per section.  The average price in 2019 overall within the 3 radius was $19/acre.</t>
-        </is>
-      </c>
-      <c r="K76" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L76" t="inlineStr">
+Liberty Petr paid between $12/acre and $19/acre, averaging at $17/acre per section.  The average price in 2019 overall within the 3 radius was $19/acre.  The highest price paid in 2019 was $22/acre</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 4 wells outside the tract within a 3 mile radius.
@@ -4630,13 +4358,10 @@
       <c r="J77" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid between $12/acre and $80/acre, averaging at $30/acre per section.  The average price in 2019 overall within the 3 radius was $30/acre.</t>
-        </is>
-      </c>
-      <c r="K77" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L77" t="inlineStr">
+Liberty Petr paid between $12/acre and $29/acre, averaging at $20/acre per section.  The average price in 2019 overall within the 3 radius was $30/acre.  The highest price paid in 2019 was $80/acre</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 5 wells outside the tract within a 3 mile radius.
@@ -4686,13 +4411,10 @@
       <c r="J78" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid between $12/acre and $80/acre, averaging at $30/acre per section.  The average price in 2019 overall within the 3 radius was $30/acre.</t>
-        </is>
-      </c>
-      <c r="K78" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L78" t="inlineStr">
+Liberty Petr paid between $12/acre and $22/acre, averaging at $18/acre per section.  The average price in 2019 overall within the 3 radius was $30/acre.  The highest price paid in 2019 was $80/acre</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4738,14 +4460,10 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Kirkwood O&amp;G paid $8/acre.  </t>
-        </is>
-      </c>
-      <c r="K79" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L79" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4791,14 +4509,10 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Baseline Minerals paid $24/acre.  </t>
-        </is>
-      </c>
-      <c r="K80" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L80" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4844,14 +4558,10 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Baseline Minerals paid $24/acre.  </t>
-        </is>
-      </c>
-      <c r="K81" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L81" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4897,14 +4607,10 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $23/acre.  </t>
-        </is>
-      </c>
-      <c r="K82" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L82" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -4951,13 +4657,10 @@
       <c r="J83" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid $32/acre.  Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.</t>
-        </is>
-      </c>
-      <c r="K83" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L83" t="inlineStr">
+Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
         <is>
           <t xml:space="preserve">There are 1 wells within the tract.
 1 wells reported production. They produced: 1 mbbl and 103 mmcf at 8280 ft from years 1996-2001
@@ -5008,13 +4711,10 @@
       <c r="J84" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid $32/acre.  Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.</t>
-        </is>
-      </c>
-      <c r="K84" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L84" t="inlineStr">
+Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -5060,14 +4760,10 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bro Energy paid $23/acre.  </t>
-        </is>
-      </c>
-      <c r="K85" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L85" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 6 wells outside the tract within a 3 mile radius.
@@ -5119,10 +4815,7 @@
           <t>There are no recorded leases within a 3 mile radius</t>
         </is>
       </c>
-      <c r="K86" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L86" t="inlineStr">
+      <c r="K86" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 4 wells outside the tract within a 3 mile radius.
@@ -5172,13 +4865,10 @@
       <c r="J87" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Liberty Petr paid between $9/acre and $18/acre, averaging at $14/acre per section.  Kirkwood O&amp;G paid $6/acre.  The average price in 2018 overall within the 3 radius was $14/acre.</t>
-        </is>
-      </c>
-      <c r="K87" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L87" t="inlineStr">
+Liberty Petr paid between $9/acre and $14/acre, averaging at $12/acre per section.  Kirkwood O&amp;G paid $6/acre.  The average price in 2018 overall within the 3 radius was $14/acre.  The highest price paid in 2018 was $18/acre</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -5225,13 +4915,10 @@
       <c r="J88" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Liberty Petr paid between $12/acre and $14/acre, averaging at $13/acre per section.  Bro Energy paid $5/acre.  The average price in 2018 overall within the 3 radius was $11/acre.</t>
-        </is>
-      </c>
-      <c r="K88" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L88" t="inlineStr">
+Liberty Petr paid $12/acre.  Bro Energy paid $5/acre.  The average price in 2018 overall within the 3 radius was $11/acre.  The highest price paid in 2018 was $14/acre</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 2 wells outside the tract within a 3 mile radius.
@@ -5281,13 +4968,10 @@
       <c r="J89" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Liberty Petr paid between $12/acre and $14/acre, averaging at $12/acre per section.  Kirkwood O&amp;G paid $6/acre.  The average price in 2018 overall within the 3 radius was $11/acre.</t>
-        </is>
-      </c>
-      <c r="K89" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L89" t="inlineStr">
+Liberty Petr paid $12/acre.  Kirkwood O&amp;G paid $6/acre.  The average price in 2018 overall within the 3 radius was $11/acre.  The highest price paid in 2018 was $14/acre</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -5334,13 +5018,10 @@
       <c r="J90" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid $32/acre.  Liberty Petr paid $12/acre.  </t>
-        </is>
-      </c>
-      <c r="K90" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L90" t="inlineStr">
+Liberty Petr paid $12/acre.  </t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 10 wells outside the tract within a 3 mile radius.
@@ -5389,14 +5070,10 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid $32/acre.  </t>
-        </is>
-      </c>
-      <c r="K91" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L91" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -5443,13 +5120,10 @@
       <c r="J92" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid $32/acre.  Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.</t>
-        </is>
-      </c>
-      <c r="K92" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L92" t="inlineStr">
+Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 19 wells outside the tract within a 3 mile radius.
@@ -5499,13 +5173,10 @@
       <c r="J93" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid $32/acre.  Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.</t>
-        </is>
-      </c>
-      <c r="K93" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L93" t="inlineStr">
+Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 11 wells outside the tract within a 3 mile radius.
@@ -5555,13 +5226,10 @@
       <c r="J94" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $4/acre and $25/acre, averaging at $8/acre per section.  Bro Energy paid $5/acre.  The average price in 2018 overall within the 3 radius was $7/acre.</t>
-        </is>
-      </c>
-      <c r="K94" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L94" t="inlineStr">
+Kirkwood O&amp;G paid between $4/acre and $7/acre, averaging at $5/acre per section.  Bro Energy paid $5/acre.  The average price in 2018 overall within the 3 radius was $7/acre.  The highest price paid in 2018 was $25/acre</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -5608,13 +5276,10 @@
       <c r="J95" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $4/acre and $25/acre, averaging at $8/acre per section.  The average price in 2018 overall within the 3 radius was $8/acre.</t>
-        </is>
-      </c>
-      <c r="K95" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L95" t="inlineStr">
+Kirkwood O&amp;G paid between $4/acre and $7/acre, averaging at $6/acre per section.  The average price in 2018 overall within the 3 radius was $8/acre.  The highest price paid in 2018 was $25/acre</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 4 wells outside the tract within a 3 mile radius.
@@ -5666,10 +5331,7 @@
           <t>There are no recorded leases within a 3 mile radius</t>
         </is>
       </c>
-      <c r="K96" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L96" t="inlineStr">
+      <c r="K96" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 2 wells outside the tract within a 3 mile radius.
@@ -5719,13 +5381,10 @@
       <c r="J97" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bro Energy paid $6/acre.  Kirkwood O&amp;G paid $3/acre.  </t>
-        </is>
-      </c>
-      <c r="K97" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L97" t="inlineStr">
+Kirkwood O&amp;G paid $3/acre.  </t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 3 wells outside the tract within a 3 mile radius.
@@ -5775,13 +5434,10 @@
       <c r="J98" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $1/acre and $5/acre, averaging at $3/acre per section.  Sitka Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $5/acre.</t>
-        </is>
-      </c>
-      <c r="K98" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L98" t="inlineStr">
+Kirkwood O&amp;G paid between $1/acre and $5/acre, averaging at $3/acre per section.  Sitka Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $5/acre.  The highest price paid in 2018 was $8/acre</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
         <is>
           <t>error occured</t>
         </is>
@@ -5828,13 +5484,10 @@
       <c r="J99" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bro Energy paid $6/acre.  Sitka Energy paid between $6/acre and $7/acre, averaging at $6/acre per section.  The average price in 2018 overall within the 3 radius was $6/acre.</t>
-        </is>
-      </c>
-      <c r="K99" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L99" t="inlineStr">
+Bro Energy paid $6/acre.  Kirkwood O&amp;G paid $3/acre.  The average price in 2018 overall within the 3 radius was $6/acre.  The highest price paid in 2018 was $7/acre</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 1 wells outside the tract within a 3 mile radius.
@@ -5884,13 +5537,10 @@
       <c r="J100" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $2/acre and $3/acre, averaging at $2/acre per section.  Bro Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $4/acre.</t>
-        </is>
-      </c>
-      <c r="K100" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L100" t="inlineStr">
+Kirkwood O&amp;G paid between $2/acre and $3/acre, averaging at $2/acre per section.  Bro Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $4/acre.  The highest price paid in 2018 was $7/acre</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -5937,13 +5587,10 @@
       <c r="J101" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $1/acre and $5/acre, averaging at $3/acre per section.  Sitka Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $5/acre.</t>
-        </is>
-      </c>
-      <c r="K101" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L101" t="inlineStr">
+Kirkwood O&amp;G paid between $1/acre and $5/acre, averaging at $3/acre per section.  Sitka Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $5/acre.  The highest price paid in 2018 was $8/acre</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
         <is>
           <t xml:space="preserve">
 There are 2 wells outside the tract within a 3 mile radius.
@@ -5994,14 +5641,10 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-O&amp;G Reservoir Development Leaders paid $12/acre.  </t>
-        </is>
-      </c>
-      <c r="K102" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L102" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -6048,13 +5691,10 @@
       <c r="J103" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood O&amp;G paid between $1/acre and $6/acre, averaging at $4/acre per section.  </t>
-        </is>
-      </c>
-      <c r="K103" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L103" t="inlineStr">
+Kirkwood O&amp;G paid $1/acre.  </t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -6101,13 +5741,10 @@
       <c r="J104" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood O&amp;G paid between $1/acre and $22/acre, averaging at $12/acre per section.  </t>
-        </is>
-      </c>
-      <c r="K104" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L104" t="inlineStr">
+Kirkwood O&amp;G paid $1/acre.  </t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -6153,14 +5790,10 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood O&amp;G paid $6/acre.  </t>
-        </is>
-      </c>
-      <c r="K105" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L105" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>
@@ -6206,14 +5839,10 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>In a 3 mile radius, the latest leases with bonus information were taken in 2016.
-Wold Oil paid $13/acre.  The average price in 2016 overall within the 3 radius was $13/acre.</t>
-        </is>
-      </c>
-      <c r="K106" s="2" t="n">
-        <v>43913</v>
-      </c>
-      <c r="L106" t="inlineStr">
+          <t>error occured</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
         <is>
           <t>No old wells within tract or in 3 mile radius of tract.</t>
         </is>

</xml_diff>

<commit_message>
added functionality to save filtered data to excel file for retrieval
</commit_message>
<xml_diff>
--- a/Results/Activity Summary Notes.xlsx
+++ b/Results/Activity Summary Notes.xlsx
@@ -459,7 +459,7 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Anderson O&amp;G paid $2/acre.  Diamond Resources paid $8/acre.  The average price in 2019 overall within the 3 radius was $145/acre.  The highest price paid in 2019 was $640/acre</t>
+Anderson O&amp;G paid between $2/acre and $640/acre.  Diamond Resources paid $8/acre.  The weighted average price in 2019 overall within the 3 radius was $157/acre.  The highest price paid in 2019 was $640/acre</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -509,12 +509,15 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Southland Royalty paid $39/acre.  The average price in 2018 overall within the 3 radius was $42/acre.  The highest price paid in 2018 was $46/acre</t>
+Southland Royalty paid between $39/acre and $46/acre.  The weighted average price in 2018 overall within the 3 radius was $42/acre.  The highest price paid in 2018 was $46/acre</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 45 wells outside the tract within a 3 mile radius.
+Out of these, 2 were dry and 33 do not have reported production. 
+The top wells that produced made: 214 mbbl and 8651 mmcf at 9557 ft in 481 months; 223 mbbl and 8217 mmcf at 9504 ft in 469 months; 85 mbbl and 4401 mmcf at 9715 ft in 325 months; 98 mbbl and 4290 mmcf at 9707 ft in 455 months; 128 mbbl and 3856 mmcf at 10170 ft in 435 months; </t>
         </is>
       </c>
     </row>
@@ -563,7 +566,8 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Western American Resources paid $640/acre.  </t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -613,7 +617,7 @@
       <c r="J5" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Edge Energy Ii paid between $53/acre and $106/acre, averaging at $85/acre per section.  Carpenter &amp; Sons paid between $1760/acre and $8960/acre, averaging at $4373/acre per section.  The average price in 2019 overall within the 3 radius was $5861/acre.  The highest price paid in 2019 was $49280/acre</t>
+Edge Energy Ii paid between $53/acre and $106/acre.  Gungnir Resources paid between $111/acre and $49280/acre.  The weighted average price in 2019 overall within the 3 radius was $4193/acre.  The highest price paid in 2019 was $49280/acre</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -662,7 +666,8 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Midland Energy paid $21/acre.  </t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -711,7 +716,8 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Robert L Bayless paid $52/acre.  The weighted average price in 2017 overall within the 3 radius was $52/acre.  </t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -760,7 +766,8 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Midland Energy paid $28/acre.  </t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -810,7 +817,7 @@
       <c r="J9" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Robert L Bayless paid between $26/acre and $28/acre, averaging at $27/acre per section.  The average price in 2017 overall within the 3 radius was $44/acre.  The highest price paid in 2017 was $52/acre</t>
+Robert L Bayless paid between $26/acre and $52/acre.  The weighted average price in 2017 overall within the 3 radius was $43/acre.  The highest price paid in 2017 was $52/acre</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -859,7 +866,8 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Midland Energy paid $28/acre.  </t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -908,7 +916,8 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Midland Energy paid $28/acre.  </t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -957,7 +966,8 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Robert L Bayless paid $8/acre.  </t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1006,7 +1016,8 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Robert L Bayless paid $8/acre.  </t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1056,7 +1067,7 @@
       <c r="J14" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Colorado Energy Minerals paid $37/acre.  </t>
+Colorado Energy Minerals paid $37/acre.  Thunder Basin Resources paid $52/acre.  </t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1105,7 +1116,8 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Colorado Energy Minerals paid $37/acre.  </t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1155,7 +1167,7 @@
       <c r="J16" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Colorado Energy Minerals paid $37/acre.  </t>
+Colorado Energy Minerals paid $37/acre.  Thunder Basin Resources paid $52/acre.  </t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1209,7 +1221,7 @@
       <c r="J17" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Rockies Resources Holding paid between $10320/acre and $30960/acre, averaging at $20640/acre per section.  The average price in 2019 overall within the 3 radius was $58133/acre.  The highest price paid in 2019 was $133120/acre</t>
+Rockies Resources Holding paid between $10320/acre and $30960/acre.  Massif O&amp;G paid $133120/acre.  The weighted average price in 2019 overall within the 3 radius was $97347/acre.  The highest price paid in 2019 was $133120/acre</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1264,7 +1276,8 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2014.
+Mbi O&amp;G paid $3100/acre.  </t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1319,7 +1332,8 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2014.
+Mbi O&amp;G paid $3100/acre.  </t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1374,7 +1388,8 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Peak Powder River Resources paid $4002/acre.  </t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1429,7 +1444,8 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1484,7 +1500,8 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1539,7 +1556,8 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1594,7 +1612,8 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -1649,7 +1668,8 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -1704,7 +1724,8 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1759,7 +1780,8 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -1814,7 +1836,8 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -1869,7 +1892,8 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -1924,7 +1948,8 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Onyx Energy paid $3052/acre.  </t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -1974,7 +1999,7 @@
       <c r="J31" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Whiskey Gulch paid $83/acre.  Langham Petr paid $208/acre.  The average price in 2019 overall within the 3 radius was $263/acre.  The highest price paid in 2019 was $708/acre</t>
+Whiskey Gulch paid between $83/acre and $708/acre.  Langham Petr paid $208/acre.  The weighted average price in 2019 overall within the 3 radius was $225/acre.  The highest price paid in 2019 was $708/acre</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2028,7 +2053,7 @@
       <c r="J32" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Renos L&amp;M paid $506/acre.  Baseline Minerals paid $1101/acre.  The average price in 2019 overall within the 3 radius was $777/acre.  The highest price paid in 2019 was $1514/acre</t>
+Renos L&amp;M paid $506/acre.  Baseline Minerals paid between $1101/acre and $1514/acre.  The weighted average price in 2019 overall within the 3 radius was $736/acre.  The highest price paid in 2019 was $1514/acre</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2078,7 +2103,7 @@
       <c r="J33" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2017.
-Kirkwood O&amp;G paid $16/acre.  The average price in 2017 overall within the 3 radius was $25/acre.  The highest price paid in 2017 was $30/acre</t>
+Stroud Expl paid $30/acre.  Kirkwood O&amp;G paid $16/acre.  The weighted average price in 2017 overall within the 3 radius was $27/acre.  The highest price paid in 2017 was $30/acre</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2134,7 +2159,7 @@
       <c r="J34" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Samson Resources paid $1526/acre.  The average price in 2019 overall within the 3 radius was $2080/acre.  The highest price paid in 2019 was $5751/acre</t>
+2323 Ss paid $302/acre.  Samson Resources paid $1526/acre.  The weighted average price in 2019 overall within the 3 radius was $1569/acre.  The highest price paid in 2019 was $5751/acre</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2190,7 +2215,7 @@
       <c r="J35" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Colorado Energy Minerals paid $2011/acre.  The average price in 2019 overall within the 3 radius was $2150/acre.  The highest price paid in 2019 was $5751/acre</t>
+2323 Ss paid $302/acre.  Titan Expl paid $5751/acre.  The weighted average price in 2019 overall within the 3 radius was $1569/acre.  The highest price paid in 2019 was $5751/acre</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2244,7 +2269,7 @@
       <c r="J36" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Colorado Energy Minerals paid $2011/acre.  The average price in 2019 overall within the 3 radius was $2150/acre.  The highest price paid in 2019 was $5751/acre</t>
+2323 Ss paid $302/acre.  Titan Expl paid $5751/acre.  The weighted average price in 2019 overall within the 3 radius was $1569/acre.  The highest price paid in 2019 was $5751/acre</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2298,7 +2323,7 @@
       <c r="J37" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-2323 Ss paid $302/acre.  Colorado Energy Minerals paid $2011/acre.  The average price in 2019 overall within the 3 radius was $3013/acre.  The highest price paid in 2019 was $5751/acre</t>
+Titan Expl paid $5751/acre.  2323 Ss paid $302/acre.  The weighted average price in 2019 overall within the 3 radius was $1575/acre.  The highest price paid in 2019 was $5751/acre</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -2353,7 +2378,8 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2013.
+Lone Tree Energy paid $570/acre.  </t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -2408,7 +2434,8 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2010.
+Southwestern Prod paid $700/acre.  </t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -2458,7 +2485,7 @@
       <c r="J40" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Knprb Leases paid $27/acre.  The average price in 2019 overall within the 3 radius was $366/acre.  The highest price paid in 2019 was $502/acre</t>
+Impact Energy paid $502/acre.  Knprb Leases paid $27/acre.  The weighted average price in 2019 overall within the 3 radius was $424/acre.  The highest price paid in 2019 was $502/acre</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -2508,7 +2535,7 @@
       <c r="J41" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Knprb Leases paid between $27/acre and $252/acre, averaging at $177/acre per section.  Bradley Williams paid $7/acre.  The average price in 2019 overall within the 3 radius was $284/acre.  The highest price paid in 2019 was $502/acre</t>
+Impact Energy paid $502/acre.  Knprb Leases paid between $27/acre and $252/acre.  The weighted average price in 2019 overall within the 3 radius was $316/acre.  The highest price paid in 2019 was $502/acre</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -2558,7 +2585,7 @@
       <c r="J42" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Percheron Professional Services paid $59/acre.  The average price in 2019 overall within the 3 radius was $67/acre.  The highest price paid in 2019 was $84/acre</t>
+Percheron Professional Services paid $59/acre.  Kirkwood Resources paid $84/acre.  The weighted average price in 2019 overall within the 3 radius was $63/acre.  The highest price paid in 2019 was $84/acre</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -2607,7 +2634,8 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Liberty Petr paid $2/acre.  The weighted average price in 2019 overall within the 3 radius was $2/acre.  </t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -2657,7 +2685,7 @@
       <c r="J44" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Rockies Resources Holding paid $640/acre.  </t>
+Mason Resources paid $788/acre.  Rockies Resources Holding paid $640/acre.  </t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -2709,12 +2737,16 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2016.
+Angelle &amp; Donohue O&amp;G paid $10/acre.  </t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 24 wells outside the tract within a 3 mile radius.
+Out of these, 4 were dry and 14 do not have reported production. 
+The top wells that produced made: 11 mbbl and 406 mmcf at 13277 ft in 155 months; 3 mbbl and 232 mmcf at 13359 ft in 154 months; 6 mbbl and 81 mmcf at 13182 ft in 108 months; 2 mbbl and 41 mmcf at 13182 ft in 109 months; 2 mbbl and 19 mmcf at 12800 ft in 29 months; </t>
         </is>
       </c>
     </row>
@@ -2760,7 +2792,7 @@
       <c r="J46" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid between $2/acre and $12/acre, averaging at $7/acre per section.  The average price in 2019 overall within the 3 radius was $11/acre.  The highest price paid in 2019 was $19/acre</t>
+Kirkwood Resources paid between $2/acre and $12/acre.  Diamond Resources paid $19/acre.  The weighted average price in 2019 overall within the 3 radius was $11/acre.  The highest price paid in 2019 was $19/acre</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -2813,7 +2845,7 @@
       <c r="J47" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $12/acre.  </t>
+Kirkwood Resources paid $12/acre.  Sitka O&amp;G paid $18/acre.  </t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -2866,7 +2898,7 @@
       <c r="J48" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Baseline Minerals paid $22/acre.  The average price in 2018 overall within the 3 radius was $22/acre.  The highest price paid in 2018 was $23/acre</t>
+Baseline Minerals paid between $22/acre and $23/acre.  The weighted average price in 2018 overall within the 3 radius was $22/acre.  The highest price paid in 2018 was $23/acre</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -2915,7 +2947,8 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Kirkwood O&amp;G paid $16/acre.  </t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -2964,7 +2997,8 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Kirkwood O&amp;G paid $16/acre.  </t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -3013,7 +3047,8 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Kirkwood Resources paid $12/acre.  </t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -3063,7 +3098,8 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Rockies Resources Holding paid $29/acre.  </t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -3112,16 +3148,16 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Hrm Resources paid $19/acre.  </t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t xml:space="preserve">There are 1 wells within the tract.
-1 wells reported production. They produced: 16 mbbl and 734 mmcf at 12145 ft from years 2006-2019
-There are 16 wells outside the tract within a 3 mile radius.
+          <t xml:space="preserve">
+There are 17 wells outside the tract within a 3 mile radius.
 Out of these, 1 were dry and 3 do not have reported production. 
-The top wells that produced made: 13 mbbl and 833 mmcf at 11450 ft in 178 months; 7 mbbl and 498 mmcf at 11862 ft in 173 months; 9 mbbl and 447 mmcf at 12350 ft in 163 months; 5 mbbl and 200 mmcf at 11750 ft in 160 months; 17 mbbl and 61 mmcf at 16420 ft in 35 months; </t>
+The top wells that produced made: 13 mbbl and 833 mmcf at 11450 ft in 178 months; 16 mbbl and 734 mmcf at 12145 ft in 113 months; 7 mbbl and 498 mmcf at 11862 ft in 173 months; 9 mbbl and 447 mmcf at 12350 ft in 163 months; 5 mbbl and 200 mmcf at 11750 ft in 160 months; </t>
         </is>
       </c>
     </row>
@@ -3168,7 +3204,7 @@
       <c r="J54" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Shadco paid $2/acre.  The average price in 2019 overall within the 3 radius was $4/acre.  The highest price paid in 2019 was $7/acre</t>
+Shadco paid between $2/acre and $7/acre.  The weighted average price in 2019 overall within the 3 radius was $4/acre.  The highest price paid in 2019 was $7/acre</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -3218,7 +3254,7 @@
       <c r="J55" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Mason Resources paid between $71/acre and $76/acre, averaging at $75/acre per section.  The average price in 2019 overall within the 3 radius was $77/acre.  The highest price paid in 2019 was $81/acre</t>
+Mason Resources paid between $71/acre and $81/acre.  The weighted average price in 2019 overall within the 3 radius was $76/acre.  The highest price paid in 2019 was $81/acre</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -3268,7 +3304,7 @@
       <c r="J56" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Prima Expl paid $23/acre.  </t>
+Prima Expl paid between $23/acre and $52/acre.  </t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -3323,12 +3359,16 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Bso paid $152/acre.  </t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 102 wells outside the tract within a 3 mile radius.
+Out of these, 2 were dry and 98 do not have reported production. 
+The top wells that produced made: 28 mbbl and 694 mmcf at 12431 ft in 7 months; 9 mbbl and 217 mmcf at 11785 ft in 6 months; </t>
         </is>
       </c>
     </row>
@@ -3373,7 +3413,7 @@
       <c r="J58" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Black Oak Energy paid between $18/acre and $28/acre, averaging at $21/acre per section.  The average price in 2018 overall within the 3 radius was $25/acre.  The highest price paid in 2018 was $58/acre</t>
+Black Oak Energy paid between $18/acre and $58/acre.  The weighted average price in 2018 overall within the 3 radius was $26/acre.  The highest price paid in 2018 was $58/acre</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -3425,12 +3465,16 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Black Oak Energy paid $50/acre.  The weighted average price in 2019 overall within the 3 radius was $50/acre.  </t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 3 wells outside the tract within a 3 mile radius.
+Out of these, 3 were dry and 0 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -3475,7 +3519,7 @@
       <c r="J60" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $26/acre.  The average price in 2019 overall within the 3 radius was $38/acre.  The highest price paid in 2019 was $50/acre</t>
+Black Oak Energy paid $50/acre.  Kirkwood Resources paid $26/acre.  The weighted average price in 2019 overall within the 3 radius was $41/acre.  The highest price paid in 2019 was $50/acre</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -3528,12 +3572,15 @@
       <c r="J61" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $26/acre.  The average price in 2019 overall within the 3 radius was $38/acre.  The highest price paid in 2019 was $50/acre</t>
+Black Oak Energy paid $50/acre.  Kirkwood Resources paid $26/acre.  The weighted average price in 2019 overall within the 3 radius was $41/acre.  The highest price paid in 2019 was $50/acre</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 36 wells outside the tract within a 3 mile radius.
+Out of these, 4 were dry and 32 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -3578,12 +3625,15 @@
       <c r="J62" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Diamond Resources paid $9/acre.  Kirkwood Resources paid $3/acre.  The average price in 2019 overall within the 3 radius was $29/acre.  The highest price paid in 2019 was $82/acre</t>
+Diamond Resources paid $9/acre.  Mason Resources paid $82/acre.  The weighted average price in 2019 overall within the 3 radius was $48/acre.  The highest price paid in 2019 was $82/acre</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 21 wells outside the tract within a 3 mile radius.
+Out of these, 17 were dry and 1 do not have reported production. 
+The top wells that produced made: 3 mbbl and 35 mmcf at 9923 ft in 42 months; 2 mbbl and 32 mmcf at 3815 ft in 28 months; </t>
         </is>
       </c>
     </row>
@@ -3627,7 +3677,8 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Diamond Resources paid $9/acre.  The weighted average price in 2019 overall within the 3 radius was $9/acre.  </t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -3681,7 +3732,7 @@
       <c r="J64" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood O&amp;G paid $19/acre.  The average price in 2019 overall within the 3 radius was $57/acre.  The highest price paid in 2019 was $76/acre</t>
+Mason Resources paid $76/acre.  Kirkwood O&amp;G paid $19/acre.  The weighted average price in 2019 overall within the 3 radius was $62/acre.  The highest price paid in 2019 was $76/acre</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -3729,7 +3780,7 @@
       <c r="I65" t="inlineStr">
         <is>
           <t xml:space="preserve">There are 4 wells within 3 mile radius that have started producing within last 4 years
-2 are V wells; 2 are D wells
+2 are D wells; 2 are V wells
 1 well has made nan mbbl and 51 mmcfd in 12 months and is currently making nan bpd and 96 mcfd.  2 wells have produced for 25 to 36 months and have made between 0 to 6 mbbls with 31 to 515 mmcf of gas.  These wells are currently averaging 1 bpd and 143 mcfd.  </t>
         </is>
       </c>
@@ -3740,7 +3791,10 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 297 wells outside the tract within a 3 mile radius.
+Out of these, 0 were dry and 35 do not have reported production. 
+The top wells that produced made: 34 mbbl and 3415 mmcf at 10688 ft in 284 months; 27 mbbl and 2603 mmcf at 10922 ft in 251 months; 16 mbbl and 2650 mmcf at 10600 ft in 262 months; 22 mbbl and 2551 mmcf at 10671 ft in 205 months; 22 mbbl and 1996 mmcf at 10956 ft in 252 months; </t>
         </is>
       </c>
     </row>
@@ -3785,12 +3839,15 @@
       <c r="J66" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood Resources paid $3/acre.  Diamond Resources paid $9/acre.  The average price in 2019 overall within the 3 radius was $17/acre.  The highest price paid in 2019 was $82/acre</t>
+Kirkwood Resources paid $3/acre.  Diamond Resources paid $9/acre.  The weighted average price in 2019 overall within the 3 radius was $48/acre.  The highest price paid in 2019 was $82/acre</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 16 wells outside the tract within a 3 mile radius.
+Out of these, 10 were dry and 1 do not have reported production. 
+The top wells that produced made: 0 mbbl and 571 mmcf at 9773 ft in 256 months; 0 mbbl and 364 mmcf at 9773 ft in 72 months; 3 mbbl and 35 mmcf at 9923 ft in 42 months; 2 mbbl and 32 mmcf at 3815 ft in 28 months; 0 mbbl and 33 mmcf at 5330 ft in 4 months; </t>
         </is>
       </c>
     </row>
@@ -3834,7 +3891,8 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Black Oak Energy paid $53/acre.  </t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -3887,12 +3945,15 @@
       <c r="J68" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Black Oak Energy paid between $52/acre and $53/acre, averaging at $53/acre per section.  Mason Resources paid $27/acre.  The average price in 2019 overall within the 3 radius was $54/acre.  The highest price paid in 2019 was $62/acre</t>
+Hrm Resources paid $62/acre.  Black Oak Energy paid between $52/acre and $53/acre.  The weighted average price in 2019 overall within the 3 radius was $50/acre.  The highest price paid in 2019 was $62/acre</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 79 wells outside the tract within a 3 mile radius.
+Out of these, 1 were dry and 77 do not have reported production. 
+The top wells that produced made: 0 mbbl and 21 mmcf at 14315 ft in 15 months; </t>
         </is>
       </c>
     </row>
@@ -3936,12 +3997,16 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Kirkwood O&amp;G paid $16/acre.  </t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 25 wells outside the tract within a 3 mile radius.
+Out of these, 2 were dry and 15 do not have reported production. 
+The top wells that produced made: 9 mbbl and 967 mmcf at 12118 ft in 191 months; 4 mbbl and 745 mmcf at 12447 ft in 185 months; 4 mbbl and 577 mmcf at 12555 ft in 162 months; 3 mbbl and 456 mmcf at 12157 ft in 142 months; 4 mbbl and 415 mmcf at 11943 ft in 194 months; </t>
         </is>
       </c>
     </row>
@@ -3986,17 +4051,15 @@
       <c r="J70" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Southland Royalty paid between $39/acre and $68/acre, averaging at $55/acre per section.  Baseline Minerals paid between $62/acre and $82/acre, averaging at $72/acre per section.  The average price in 2018 overall within the 3 radius was $77/acre.  The highest price paid in 2018 was $108/acre</t>
+Southland Royalty paid between $39/acre and $108/acre.  Baseline Minerals paid between $62/acre and $82/acre.  The weighted average price in 2018 overall within the 3 radius was $69/acre.  The highest price paid in 2018 was $108/acre</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t xml:space="preserve">There are 3 wells within the tract.
-1 dry holes in tract.
-2 wells reported production. They produced: 2 mbbl and 348 mmcf at 8650 ft from years 1996-2012 They produced: 1 mbbl and 150 mmcf at 8454 ft from years 1979-1989
-There are 5 wells outside the tract within a 3 mile radius.
-Out of these, 2 were dry and 1 do not have reported production. 
-The top wells that produced made: 4 mbbl and 818 mmcf at 8750 ft in 400 months; 3 mbbl and 221 mmcf at 8913 ft in 151 months; </t>
+          <t xml:space="preserve">
+There are 8 wells outside the tract within a 3 mile radius.
+Out of these, 3 were dry and 1 do not have reported production. 
+The top wells that produced made: 4 mbbl and 818 mmcf at 8750 ft in 400 months; 2 mbbl and 348 mmcf at 8650 ft in 144 months; 3 mbbl and 221 mmcf at 8913 ft in 151 months; 1 mbbl and 150 mmcf at 8454 ft in 90 months; </t>
         </is>
       </c>
     </row>
@@ -4041,7 +4104,7 @@
       <c r="J71" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid between $28/acre and $39/acre, averaging at $32/acre per section.  Black Oak Energy paid $50/acre.  The average price in 2019 overall within the 3 radius was $40/acre.  The highest price paid in 2019 was $52/acre</t>
+Liberty Petr paid between $28/acre and $39/acre.  Black Oak Energy paid between $50/acre and $52/acre.  The weighted average price in 2019 overall within the 3 radius was $39/acre.  The highest price paid in 2019 was $52/acre</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -4096,14 +4159,13 @@
       <c r="J72" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Southland Royalty paid between $36/acre and $67/acre, averaging at $45/acre per section.  The average price in 2018 overall within the 3 radius was $57/acre.  The highest price paid in 2018 was $94/acre</t>
+Southland Royalty paid between $36/acre and $67/acre.  Baseline Minerals paid $94/acre.  The weighted average price in 2018 overall within the 3 radius was $61/acre.  The highest price paid in 2018 was $94/acre</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t xml:space="preserve">There are 1 wells within the tract.
-1 wells reported production. They produced: 11 mbbl and 3659 mmcf at 6579 ft from years 1974-2016
-There are 46 wells outside the tract within a 3 mile radius.
+          <t xml:space="preserve">
+There are 47 wells outside the tract within a 3 mile radius.
 Out of these, 9 were dry and 5 do not have reported production. 
 The top wells that produced made: 51 mbbl and 16413 mmcf at 6510 ft in 528 months; 17 mbbl and 12633 mmcf at 6015 ft in 528 months; 14 mbbl and 12534 mmcf at 6209 ft in 407 months; 49 mbbl and 10992 mmcf at 5635 ft in 538 months; 44 mbbl and 10229 mmcf at 6838 ft in 541 months; </t>
         </is>
@@ -4149,12 +4211,16 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Kirkwood Resources paid $2/acre.  </t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 17 wells outside the tract within a 3 mile radius.
+Out of these, 9 were dry and 6 do not have reported production. 
+The top wells that produced made: 7 mbbl and 2011 mmcf at 5325 ft in 236 months; 1 mbbl and 219 mmcf at 5528 ft in 155 months; </t>
         </is>
       </c>
     </row>
@@ -4198,14 +4264,14 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2014.
+Teton Resources paid $18/acre.  </t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t xml:space="preserve">There are 1 wells within the tract.
-1 wells reported production. They produced: 0 mbbl and 374 mmcf at 11450 ft from years 2002-2018
-There are 23 wells outside the tract within a 3 mile radius.
+          <t xml:space="preserve">
+There are 24 wells outside the tract within a 3 mile radius.
 Out of these, 5 were dry and 3 do not have reported production. 
 The top wells that produced made: 5 mbbl and 1297 mmcf at 10250 ft in 163 months; 1 mbbl and 1253 mmcf at 11230 ft in 194 months; 1 mbbl and 1171 mmcf at 11193 ft in 175 months; 2 mbbl and 981 mmcf at 10650 ft in 135 months; 1 mbbl and 842 mmcf at 11420 ft in 146 months; </t>
         </is>
@@ -4252,7 +4318,7 @@
       <c r="J75" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Black Oak Energy paid between $11/acre and $12/acre, averaging at $12/acre per section.  The average price in 2018 overall within the 3 radius was $17/acre.  The highest price paid in 2018 was $24/acre</t>
+Black Oak Energy paid between $11/acre and $24/acre.  The weighted average price in 2018 overall within the 3 radius was $14/acre.  The highest price paid in 2018 was $24/acre</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -4305,7 +4371,7 @@
       <c r="J76" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid between $12/acre and $19/acre, averaging at $17/acre per section.  The average price in 2019 overall within the 3 radius was $19/acre.  The highest price paid in 2019 was $22/acre</t>
+Liberty Petr paid between $12/acre and $22/acre.  The weighted average price in 2019 overall within the 3 radius was $17/acre.  The highest price paid in 2019 was $22/acre</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -4358,7 +4424,7 @@
       <c r="J77" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid between $12/acre and $29/acre, averaging at $20/acre per section.  The average price in 2019 overall within the 3 radius was $30/acre.  The highest price paid in 2019 was $80/acre</t>
+Liberty Petr paid between $12/acre and $80/acre.  The weighted average price in 2019 overall within the 3 radius was $32/acre.  The highest price paid in 2019 was $80/acre</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -4411,12 +4477,15 @@
       <c r="J78" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Liberty Petr paid between $12/acre and $22/acre, averaging at $18/acre per section.  The average price in 2019 overall within the 3 radius was $30/acre.  The highest price paid in 2019 was $80/acre</t>
+Liberty Petr paid between $12/acre and $80/acre.  The weighted average price in 2019 overall within the 3 radius was $34/acre.  The highest price paid in 2019 was $80/acre</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 4 wells outside the tract within a 3 mile radius.
+Out of these, 2 were dry and 1 do not have reported production. 
+The top wells that produced made: 0 mbbl and 41 mmcf at 12670 ft in 101 months; </t>
         </is>
       </c>
     </row>
@@ -4460,12 +4529,16 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+Kirkwood O&amp;G paid $8/acre.  </t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 4 wells outside the tract within a 3 mile radius.
+Out of these, 4 were dry and 0 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -4509,12 +4582,16 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Baseline Minerals paid $24/acre.  </t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 7 wells outside the tract within a 3 mile radius.
+Out of these, 7 were dry and 0 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -4558,12 +4635,16 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Baseline Minerals paid $24/acre.  </t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 10 wells outside the tract within a 3 mile radius.
+Out of these, 10 were dry and 0 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -4607,12 +4688,16 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Kirkwood Resources paid $23/acre.  </t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 19 wells outside the tract within a 3 mile radius.
+Out of these, 13 were dry and 2 do not have reported production. 
+The top wells that produced made: 4 mbbl and 4007 mmcf at 4633 ft in 400 months; 0 mbbl and 711 mmcf at 4633 ft in 148 months; 0 mbbl and 218 mmcf at 4545 ft in 56 months; 0 mbbl and 169 mmcf at 4545 ft in 103 months; </t>
         </is>
       </c>
     </row>
@@ -4657,14 +4742,13 @@
       <c r="J83" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
+Kirkwood O&amp;G paid $32/acre.  Bro Energy paid $23/acre.  The weighted average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t xml:space="preserve">There are 1 wells within the tract.
-1 wells reported production. They produced: 1 mbbl and 103 mmcf at 8280 ft from years 1996-2001
-There are 26 wells outside the tract within a 3 mile radius.
+          <t xml:space="preserve">
+There are 27 wells outside the tract within a 3 mile radius.
 Out of these, 8 were dry and 7 do not have reported production. 
 The top wells that produced made: 93 mbbl and 3662 mmcf at 7845 ft in 191 months; 89 mbbl and 3348 mmcf at 6840 ft in 183 months; 49 mbbl and 3351 mmcf at 6900 ft in 138 months; 88 mbbl and 3001 mmcf at 6860 ft in 213 months; 45 mbbl and 2885 mmcf at 6900 ft in 111 months; </t>
         </is>
@@ -4711,12 +4795,15 @@
       <c r="J84" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
+Kirkwood O&amp;G paid $32/acre.  Bro Energy paid $23/acre.  The weighted average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 24 wells outside the tract within a 3 mile radius.
+Out of these, 9 were dry and 3 do not have reported production. 
+The top wells that produced made: 93 mbbl and 3662 mmcf at 7845 ft in 191 months; 89 mbbl and 3348 mmcf at 6840 ft in 183 months; 49 mbbl and 3351 mmcf at 6900 ft in 138 months; 88 mbbl and 3001 mmcf at 6860 ft in 213 months; 45 mbbl and 2885 mmcf at 6900 ft in 111 months; </t>
         </is>
       </c>
     </row>
@@ -4760,7 +4847,8 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Bro Energy paid $23/acre.  </t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -4865,12 +4953,15 @@
       <c r="J87" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Liberty Petr paid between $9/acre and $14/acre, averaging at $12/acre per section.  Kirkwood O&amp;G paid $6/acre.  The average price in 2018 overall within the 3 radius was $14/acre.  The highest price paid in 2018 was $18/acre</t>
+Liberty Petr paid between $9/acre and $18/acre.  Kirkwood O&amp;G paid $6/acre.  The weighted average price in 2018 overall within the 3 radius was $13/acre.  The highest price paid in 2018 was $18/acre</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 5 wells outside the tract within a 3 mile radius.
+Out of these, 3 were dry and 2 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -4915,7 +5006,7 @@
       <c r="J88" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Liberty Petr paid $12/acre.  Bro Energy paid $5/acre.  The average price in 2018 overall within the 3 radius was $11/acre.  The highest price paid in 2018 was $14/acre</t>
+Liberty Petr paid between $12/acre and $14/acre.  Bro Energy paid $5/acre.  The weighted average price in 2018 overall within the 3 radius was $11/acre.  The highest price paid in 2018 was $14/acre</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -4968,12 +5059,15 @@
       <c r="J89" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Liberty Petr paid $12/acre.  Kirkwood O&amp;G paid $6/acre.  The average price in 2018 overall within the 3 radius was $11/acre.  The highest price paid in 2018 was $14/acre</t>
+Liberty Petr paid between $12/acre and $14/acre.  Kirkwood O&amp;G paid $6/acre.  The weighted average price in 2018 overall within the 3 radius was $12/acre.  The highest price paid in 2018 was $14/acre</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 9 wells outside the tract within a 3 mile radius.
+Out of these, 3 were dry and 6 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -5018,7 +5112,7 @@
       <c r="J90" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Liberty Petr paid $12/acre.  </t>
+Kirkwood O&amp;G paid $32/acre.  Liberty Petr paid $12/acre.  </t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -5070,12 +5164,16 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
+Kirkwood O&amp;G paid $32/acre.  </t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 12 wells outside the tract within a 3 mile radius.
+Out of these, 3 were dry and 7 do not have reported production. 
+The top wells that produced made: 15 mbbl and 365 mmcf at 7924 ft in 67 months; 1 mbbl and 103 mmcf at 8280 ft in 26 months; </t>
         </is>
       </c>
     </row>
@@ -5120,7 +5218,7 @@
       <c r="J92" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
+Kirkwood O&amp;G paid $32/acre.  Bro Energy paid $23/acre.  The weighted average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -5173,7 +5271,7 @@
       <c r="J93" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bro Energy paid $23/acre.  The average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
+Kirkwood O&amp;G paid $32/acre.  Bro Energy paid $23/acre.  The weighted average price in 2018 overall within the 3 radius was $29/acre.  The highest price paid in 2018 was $32/acre</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
@@ -5226,12 +5324,15 @@
       <c r="J94" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $4/acre and $7/acre, averaging at $5/acre per section.  Bro Energy paid $5/acre.  The average price in 2018 overall within the 3 radius was $7/acre.  The highest price paid in 2018 was $25/acre</t>
+Kirkwood O&amp;G paid between $4/acre and $25/acre.  Bro Energy paid $5/acre.  The weighted average price in 2018 overall within the 3 radius was $8/acre.  The highest price paid in 2018 was $25/acre</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 5 wells outside the tract within a 3 mile radius.
+Out of these, 5 were dry and 0 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -5276,7 +5377,7 @@
       <c r="J95" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $4/acre and $7/acre, averaging at $6/acre per section.  The average price in 2018 overall within the 3 radius was $8/acre.  The highest price paid in 2018 was $25/acre</t>
+Kirkwood O&amp;G paid between $4/acre and $25/acre.  The weighted average price in 2018 overall within the 3 radius was $7/acre.  The highest price paid in 2018 was $25/acre</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -5381,7 +5482,7 @@
       <c r="J97" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid $3/acre.  </t>
+Bro Energy paid $6/acre.  Kirkwood O&amp;G paid $3/acre.  </t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -5434,12 +5535,15 @@
       <c r="J98" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $1/acre and $5/acre, averaging at $3/acre per section.  Sitka Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $5/acre.  The highest price paid in 2018 was $8/acre</t>
+Kirkwood O&amp;G paid between $1/acre and $5/acre.  Sitka Energy paid $6/acre.  The weighted average price in 2018 overall within the 3 radius was $6/acre.  The highest price paid in 2018 was $8/acre</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">
+There are 4 wells outside the tract within a 3 mile radius.
+Out of these, 4 were dry and 0 do not have reported production. 
+</t>
         </is>
       </c>
     </row>
@@ -5484,7 +5588,7 @@
       <c r="J99" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Bro Energy paid $6/acre.  Kirkwood O&amp;G paid $3/acre.  The average price in 2018 overall within the 3 radius was $6/acre.  The highest price paid in 2018 was $7/acre</t>
+Bro Energy paid $6/acre.  Sitka Energy paid between $6/acre and $7/acre.  The weighted average price in 2018 overall within the 3 radius was $6/acre.  The highest price paid in 2018 was $7/acre</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
@@ -5537,7 +5641,7 @@
       <c r="J100" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $2/acre and $3/acre, averaging at $2/acre per section.  Bro Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $4/acre.  The highest price paid in 2018 was $7/acre</t>
+Kirkwood O&amp;G paid between $2/acre and $3/acre.  Bro Energy paid $6/acre.  The weighted average price in 2018 overall within the 3 radius was $5/acre.  The highest price paid in 2018 was $7/acre</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
@@ -5587,7 +5691,7 @@
       <c r="J101" t="inlineStr">
         <is>
           <t>In a 3 mile radius, the latest leases with bonus information were taken in 2018.
-Kirkwood O&amp;G paid between $1/acre and $5/acre, averaging at $3/acre per section.  Sitka Energy paid $6/acre.  The average price in 2018 overall within the 3 radius was $5/acre.  The highest price paid in 2018 was $8/acre</t>
+Kirkwood O&amp;G paid between $1/acre and $5/acre.  Sitka Energy paid $6/acre.  The weighted average price in 2018 overall within the 3 radius was $5/acre.  The highest price paid in 2018 was $8/acre</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
@@ -5641,7 +5745,8 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2017.
+O&amp;G Reservoir Development Leaders paid $12/acre.  </t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -5691,7 +5796,7 @@
       <c r="J103" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood O&amp;G paid $1/acre.  </t>
+Kirkwood O&amp;G paid between $1/acre and $6/acre.  </t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -5741,7 +5846,7 @@
       <c r="J104" t="inlineStr">
         <is>
           <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
-Kirkwood O&amp;G paid $1/acre.  </t>
+Kirkwood O&amp;G paid between $1/acre and $22/acre.  </t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -5790,7 +5895,8 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2019.
+Kirkwood O&amp;G paid $6/acre.  </t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -5839,7 +5945,8 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>error occured</t>
+          <t xml:space="preserve">In a 3 mile radius, the latest leases with bonus information were taken in 2016.
+Wold Oil paid $13/acre.  The weighted average price in 2016 overall within the 3 radius was $13/acre.  </t>
         </is>
       </c>
       <c r="K106" t="inlineStr">

</xml_diff>